<commit_message>
Menús agregados a Render
</commit_message>
<xml_diff>
--- a/Mapa de menus xy.xlsx
+++ b/Mapa de menus xy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x15 xr">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="164011"/>
-  <xr:revisionPtr revIDLastSave="1558" documentId="{304A662A-9121-427F-B70B-87D92418AD88}"/>
+  <xr:revisionPtr revIDLastSave="1563" documentId="{304A662A-9121-427F-B70B-87D92418AD88}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr" xr:uid="{5AFA9771-E90B-4445-8C0B-1F09B2043B6C}">
   <dimension ref="A1:CC335"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A218" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AS243" sqref="AS243"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A168" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E178" sqref="E178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -28464,7 +28464,7 @@
         <v>24</v>
       </c>
       <c r="AQ208" s="11" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="AR208" s="11" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Culminación del menú login
</commit_message>
<xml_diff>
--- a/Mapa de menus xy.xlsx
+++ b/Mapa de menus xy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x15 xr">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="164011"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="{12FBF147-BE15-437B-A0FD-C93FC81AD2F6}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="{12FBF147-BE15-437B-A0FD-C93FC81AD2F6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6592" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6586" uniqueCount="100">
   <si>
     <t>xy</t>
   </si>
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr" xr:uid="{5AFA9771-E90B-4445-8C0B-1F09B2043B6C}">
   <dimension ref="A1:CC335"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A78" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AQ105" sqref="AQ105"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Z50" sqref="Z50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -6856,97 +6856,81 @@
       <c r="T50" s="26"/>
       <c r="U50" s="26"/>
       <c r="V50" s="26"/>
-      <c r="W50" s="7" t="s">
+      <c r="AA50" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="X50" s="7" t="s">
+      <c r="AB50" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="Y50" s="7" t="s">
+      <c r="AC50" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Z50" s="7" t="s">
+      <c r="AD50" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AA50" s="7" t="s">
+      <c r="AE50" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AB50" s="7" t="s">
+      <c r="AF50" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AC50" s="7" t="s">
+      <c r="AG50" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AD50" s="7" t="s">
+      <c r="AH50" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AE50" s="7"/>
-      <c r="AF50" s="7" t="s">
+      <c r="AI50" s="7"/>
+      <c r="AJ50" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AG50" s="7" t="s">
+      <c r="AK50" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AH50" s="7" t="s">
+      <c r="AL50" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="AI50" s="7" t="s">
+      <c r="AM50" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AJ50" s="7" t="s">
+      <c r="AN50" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AK50" s="7"/>
-      <c r="AL50" s="7" t="s">
+      <c r="AO50" s="7"/>
+      <c r="AP50" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AM50" s="7" t="s">
+      <c r="AQ50" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AN50" s="7" t="s">
+      <c r="AR50" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AO50" s="7" t="s">
+      <c r="AS50" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AP50" s="7"/>
-      <c r="AQ50" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR50" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="AS50" s="7" t="s">
+      <c r="AT50" s="7"/>
+      <c r="AU50" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AV50" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW50" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AT50" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU50" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="AV50" s="7" t="s">
+      <c r="AX50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY50" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AW50" s="7"/>
-      <c r="AX50" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AY50" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="AZ50" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="BA50" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="BB50" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="BC50" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="BA50" s="7"/>
+      <c r="BB50" s="7"/>
+      <c r="BC50" s="7"/>
       <c r="BD50" s="26"/>
       <c r="BE50" s="26"/>
       <c r="BF50" s="26"/>

</xml_diff>

<commit_message>
Deploy Ready Alpha 0.7
</commit_message>
<xml_diff>
--- a/Mapa de menus xy.xlsx
+++ b/Mapa de menus xy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13407" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13407" uniqueCount="129">
   <si>
     <t>xy</t>
   </si>
@@ -1428,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr" xr:uid="{5AFA9771-E90B-4445-8C0B-1F09B2043B6C}">
   <dimension ref="A1:CC440"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F115" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="W128" sqref="W128"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A147" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I164" sqref="I164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -60852,7 +60852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr" xr:uid="{54037143-65CE-4338-B2F8-7F51CE8ECA44}">
   <dimension ref="A1:CC226"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A81" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A110" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="Y129" sqref="Y129"/>
     </sheetView>
   </sheetViews>

</xml_diff>